<commit_message>
updating tables to match schema
</commit_message>
<xml_diff>
--- a/Excel Files for Table/Agent.xlsx
+++ b/Excel Files for Table/Agent.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anime\FinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anime\FinalProject\Excel Files for Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7648496B-D75A-4E1C-9D77-7286D907380D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2991A863-3028-4A89-9ABC-FAECBC629605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="1164" windowWidth="17280" windowHeight="10620" xr2:uid="{48F9B1F7-D7B4-430E-8126-43FD56247073}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{48F9B1F7-D7B4-430E-8126-43FD56247073}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>agent_id</t>
   </si>
@@ -56,10 +56,19 @@
     <t>Melissa</t>
   </si>
   <si>
-    <t>melissa@gmail.com</t>
-  </si>
-  <si>
     <t>hello123</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>melissa@renting.com</t>
+  </si>
+  <si>
+    <t>jack@renting.com</t>
+  </si>
+  <si>
+    <t>hbye123</t>
   </si>
 </sst>
 </file>
@@ -422,14 +431,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8784BBD1-FF4C-436B-A757-22D827B446BD}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="3" max="3" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -458,18 +468,36 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>2671112233</v>
       </c>
       <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>789101</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>2158889999</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{E612A89E-0FDC-49AD-B6AA-5B690A1495C1}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{A277488B-D76C-4694-B93A-D53CD9E81065}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>